<commit_message>
edit company and consultant
edit company and consultant
</commit_message>
<xml_diff>
--- a/hrdesktop/dispatch/HPSConsultant/コンサルテントテンプレート.xlsx
+++ b/hrdesktop/dispatch/HPSConsultant/コンサルテントテンプレート.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gun\Documents\GitHub\highwayns\hrdesktop\dispatch\HPSConsultant\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095"/>
   </bookViews>
@@ -10,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$T$31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$R$31</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -24,9 +29,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
-    <t>1. 会社名</t>
-  </si>
-  <si>
     <t>2. 部署名</t>
   </si>
   <si>
@@ -76,13 +78,29 @@
   </si>
   <si>
     <t>18. 設定されたラベルの項目</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>会社名</t>
+    </r>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +121,13 @@
       <color theme="1"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="2">
@@ -136,7 +161,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -406,7 +431,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -414,139 +439,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:T18"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="C1" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="1.625" customWidth="1"/>
-    <col min="2" max="2" width="22.25" customWidth="1"/>
-    <col min="3" max="4" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.875" customWidth="1"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.875" customWidth="1"/>
+    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18" customWidth="1"/>
-    <col min="17" max="17" width="34.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25.375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="32.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" customWidth="1"/>
+    <col min="15" max="15" width="34.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="3:20" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="3:20" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="3:20" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="3:20" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="3:20" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="3:20" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="3:20" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="3:20" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="3:20" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="3:20" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="3:20" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="3:20" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="3:20" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="3:20" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="3:20" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="3:3" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="3:3" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="C18" s="1"/>
+    </row>
+    <row r="2" spans="1:18" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" spans="1:18" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:18" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:18" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:18" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:18" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:18" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:18" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:18" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:18" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:18" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:18" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:18" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:18" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:18" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A18" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>